<commit_message>
Created a table and extracted data from excel sheet
</commit_message>
<xml_diff>
--- a/Invoices/10001-2023.1.18.xlsx
+++ b/Invoices/10001-2023.1.18.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView windowWidth="23040" windowHeight="9120"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>product_id</t>
   </si>
@@ -43,34 +59,180 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -80,17 +242,203 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
-        <bgColor auto="1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="12"/>
-        <bgColor auto="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -203,77 +551,422 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00BDC0BF"/>
+      <rgbColor rgb="00A5A5A5"/>
+      <rgbColor rgb="003F3F3F"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -472,8 +1165,6 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
@@ -493,8 +1184,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -523,8 +1213,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -549,8 +1238,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -575,8 +1263,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -601,8 +1288,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -627,8 +1313,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -653,8 +1338,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -679,8 +1363,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -705,8 +1388,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -731,8 +1413,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -745,9 +1426,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -761,8 +1448,6 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
@@ -782,8 +1467,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -808,8 +1492,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -834,8 +1517,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -860,8 +1542,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -886,8 +1567,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -912,8 +1592,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -938,8 +1617,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -964,8 +1642,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -990,8 +1667,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1016,8 +1692,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1030,9 +1705,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1043,8 +1724,6 @@
           <a:noFill/>
           <a:miter lim="400000"/>
         </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
@@ -1064,8 +1743,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1094,8 +1772,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1120,8 +1797,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1146,8 +1822,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1172,8 +1847,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1198,8 +1872,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1224,8 +1897,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1250,8 +1922,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1276,8 +1947,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1302,8 +1972,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1316,9 +1985,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
@@ -1327,43 +2002,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.3333333333333" defaultRowHeight="13.9" customHeight="1" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="16.3518518518519" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.7" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" ht="14.7" customHeight="1" spans="1:6">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" ht="14.7" customHeight="1">
-      <c r="A2" t="s" s="4">
+    <row r="2" ht="14.7" customHeight="1" spans="1:6">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="6">
@@ -1377,11 +2053,11 @@
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" ht="26.7" customHeight="1">
-      <c r="A3" t="s" s="8">
+    <row r="3" ht="26.7" customHeight="1" spans="1:6">
+      <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s" s="9">
+      <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="10">
@@ -1395,7 +2071,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" ht="14.35" customHeight="1">
+    <row r="4" ht="14.35" customHeight="1" spans="1:6">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -1403,7 +2079,7 @@
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" ht="14.05" customHeight="1">
+    <row r="5" ht="14.05" customHeight="1" spans="1:6">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -1411,7 +2087,7 @@
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" ht="14.05" customHeight="1">
+    <row r="6" ht="14.05" customHeight="1" spans="1:6">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -1419,7 +2095,7 @@
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" ht="14.05" customHeight="1">
+    <row r="7" ht="14.05" customHeight="1" spans="1:6">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -1427,7 +2103,7 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" ht="14.05" customHeight="1">
+    <row r="8" ht="14.05" customHeight="1" spans="1:6">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -1435,7 +2111,7 @@
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" ht="14.05" customHeight="1">
+    <row r="9" ht="14.05" customHeight="1" spans="1:6">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -1443,7 +2119,7 @@
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" ht="14.05" customHeight="1">
+    <row r="10" ht="14.05" customHeight="1" spans="1:6">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -1453,7 +2129,7 @@
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>